<commit_message>
funzionamento efficace di euramet data
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -6571,7 +6571,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G29" s="419" t="n">
         <v>-1.1772</v>
@@ -6638,7 +6638,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G30" s="339" t="n">
         <v>-1.1772</v>
@@ -6705,10 +6705,10 @@
         <v>0</v>
       </c>
       <c r="F31" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G31" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H31" s="422" t="n">
         <v>1</v>
@@ -6839,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G33" s="339" t="n">
         <v>-1.1772</v>
@@ -6906,7 +6906,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G34" s="339" t="n">
         <v>-1.3734</v>
@@ -7043,7 +7043,7 @@
         <v>-157.0411782090434</v>
       </c>
       <c r="G36" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H36" s="426" t="n">
         <v>1</v>
@@ -7107,7 +7107,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G37" s="344" t="n">
         <v>-1.3734</v>
@@ -7177,7 +7177,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G38" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H38" s="426" t="n">
         <v>1</v>
@@ -7241,7 +7241,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G39" s="344" t="n">
         <v>-1.1772</v>
@@ -7308,10 +7308,10 @@
         <v>0</v>
       </c>
       <c r="F40" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G40" s="344" t="n">
-        <v>-1.1772</v>
+        <v>-1.3734</v>
       </c>
       <c r="H40" s="426" t="n">
         <v>1</v>
@@ -7576,10 +7576,10 @@
         <v>0</v>
       </c>
       <c r="F44" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G44" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H44" s="426" t="n">
         <v>1</v>
@@ -7639,10 +7639,18 @@
         <v/>
       </c>
       <c r="D45" s="425" t="n"/>
-      <c r="E45" s="344" t="n"/>
-      <c r="F45" s="344" t="n"/>
-      <c r="G45" s="344" t="n"/>
-      <c r="H45" s="426" t="n"/>
+      <c r="E45" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G45" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H45" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I45" s="365">
         <f>(H45-$E$27)+$H$2</f>
         <v/>
@@ -7698,10 +7706,18 @@
         <v/>
       </c>
       <c r="D46" s="425" t="n"/>
-      <c r="E46" s="344" t="n"/>
-      <c r="F46" s="344" t="n"/>
-      <c r="G46" s="344" t="n"/>
-      <c r="H46" s="426" t="n"/>
+      <c r="E46" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G46" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H46" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I46" s="366">
         <f>(H46-$E$27)+$H$2</f>
         <v/>

</xml_diff>

<commit_message>
completato operazione con un quadrante
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -6566,12 +6566,14 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n"/>
+      <c r="D29" s="418" t="n">
+        <v>837</v>
+      </c>
       <c r="E29" s="419" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G29" s="419" t="n">
         <v>-1.1772</v>
@@ -6633,15 +6635,17 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n"/>
+      <c r="D30" s="421" t="n">
+        <v>837</v>
+      </c>
       <c r="E30" s="339" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G30" s="339" t="n">
-        <v>-1.1772</v>
+        <v>-1.3734</v>
       </c>
       <c r="H30" s="422" t="n">
         <v>1</v>
@@ -6700,7 +6704,9 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n"/>
+      <c r="D31" s="421" t="n">
+        <v>837</v>
+      </c>
       <c r="E31" s="339" t="n">
         <v>0</v>
       </c>
@@ -6767,7 +6773,9 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n"/>
+      <c r="D32" s="421" t="n">
+        <v>837</v>
+      </c>
       <c r="E32" s="339" t="n">
         <v>0</v>
       </c>
@@ -6775,7 +6783,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G32" s="339" t="n">
-        <v>-1.1772</v>
+        <v>-1.3734</v>
       </c>
       <c r="H32" s="422" t="n">
         <v>1</v>
@@ -6834,7 +6842,9 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n"/>
+      <c r="D33" s="421" t="n">
+        <v>837</v>
+      </c>
       <c r="E33" s="339" t="n">
         <v>0</v>
       </c>
@@ -6901,12 +6911,14 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n"/>
+      <c r="D34" s="421" t="n">
+        <v>837</v>
+      </c>
       <c r="E34" s="339" t="n">
         <v>0</v>
       </c>
       <c r="F34" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G34" s="339" t="n">
         <v>-1.3734</v>
@@ -6968,12 +6980,14 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n"/>
+      <c r="D35" s="423" t="n">
+        <v>837</v>
+      </c>
       <c r="E35" s="343" t="n">
         <v>0</v>
       </c>
       <c r="F35" s="343" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G35" s="343" t="n">
         <v>-1.1772</v>
@@ -7035,12 +7049,14 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n"/>
+      <c r="D36" s="425" t="n">
+        <v>837</v>
+      </c>
       <c r="E36" s="344" t="n">
         <v>0</v>
       </c>
       <c r="F36" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G36" s="344" t="n">
         <v>-1.1772</v>
@@ -7102,15 +7118,17 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n"/>
+      <c r="D37" s="425" t="n">
+        <v>837</v>
+      </c>
       <c r="E37" s="344" t="n">
         <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G37" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H37" s="426" t="n">
         <v>1</v>
@@ -7170,18 +7188,10 @@
         <v/>
       </c>
       <c r="D38" s="425" t="n"/>
-      <c r="E38" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G38" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H38" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E38" s="344" t="n"/>
+      <c r="F38" s="344" t="n"/>
+      <c r="G38" s="344" t="n"/>
+      <c r="H38" s="426" t="n"/>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7237,18 +7247,10 @@
         <v/>
       </c>
       <c r="D39" s="425" t="n"/>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7304,18 +7306,10 @@
         <v/>
       </c>
       <c r="D40" s="425" t="n"/>
-      <c r="E40" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G40" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H40" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E40" s="344" t="n"/>
+      <c r="F40" s="344" t="n"/>
+      <c r="G40" s="344" t="n"/>
+      <c r="H40" s="426" t="n"/>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7371,18 +7365,10 @@
         <v/>
       </c>
       <c r="D41" s="423" t="n"/>
-      <c r="E41" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G41" s="343" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H41" s="424" t="n">
-        <v>1</v>
-      </c>
+      <c r="E41" s="343" t="n"/>
+      <c r="F41" s="343" t="n"/>
+      <c r="G41" s="343" t="n"/>
+      <c r="H41" s="424" t="n"/>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -7438,18 +7424,10 @@
         <v/>
       </c>
       <c r="D42" s="425" t="n"/>
-      <c r="E42" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G42" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H42" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E42" s="344" t="n"/>
+      <c r="F42" s="344" t="n"/>
+      <c r="G42" s="344" t="n"/>
+      <c r="H42" s="426" t="n"/>
       <c r="I42" s="365">
         <f>(H42-$E$27)+$H$2</f>
         <v/>
@@ -7505,18 +7483,10 @@
         <v/>
       </c>
       <c r="D43" s="425" t="n"/>
-      <c r="E43" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G43" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H43" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E43" s="344" t="n"/>
+      <c r="F43" s="344" t="n"/>
+      <c r="G43" s="344" t="n"/>
+      <c r="H43" s="426" t="n"/>
       <c r="I43" s="365">
         <f>(H43-$E$27)+$H$2</f>
         <v/>
@@ -7572,18 +7542,10 @@
         <v/>
       </c>
       <c r="D44" s="425" t="n"/>
-      <c r="E44" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G44" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H44" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E44" s="344" t="n"/>
+      <c r="F44" s="344" t="n"/>
+      <c r="G44" s="344" t="n"/>
+      <c r="H44" s="426" t="n"/>
       <c r="I44" s="365">
         <f>(H44-$E$27)+$H$2</f>
         <v/>
@@ -7639,18 +7601,10 @@
         <v/>
       </c>
       <c r="D45" s="425" t="n"/>
-      <c r="E45" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G45" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H45" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E45" s="344" t="n"/>
+      <c r="F45" s="344" t="n"/>
+      <c r="G45" s="344" t="n"/>
+      <c r="H45" s="426" t="n"/>
       <c r="I45" s="365">
         <f>(H45-$E$27)+$H$2</f>
         <v/>
@@ -7706,18 +7660,10 @@
         <v/>
       </c>
       <c r="D46" s="425" t="n"/>
-      <c r="E46" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G46" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H46" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="E46" s="344" t="n"/>
+      <c r="F46" s="344" t="n"/>
+      <c r="G46" s="344" t="n"/>
+      <c r="H46" s="426" t="n"/>
       <c r="I46" s="366">
         <f>(H46-$E$27)+$H$2</f>
         <v/>

</xml_diff>

<commit_message>
provare se funziona il processo di inversione quadrnate
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -5312,16 +5312,16 @@
         <v>837</v>
       </c>
       <c r="E7" s="419" t="n">
-        <v>989</v>
+        <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-0.3</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-2.4</v>
+        <v>-1.1772</v>
       </c>
       <c r="H7" s="420" t="n">
-        <v>2.42215</v>
+        <v>1</v>
       </c>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
@@ -5381,16 +5381,16 @@
         <v>837</v>
       </c>
       <c r="E8" s="339" t="n">
-        <v>883</v>
+        <v>0</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>257</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G8" s="339" t="n">
-        <v>-253.9</v>
+        <v>-1.1772</v>
       </c>
       <c r="H8" s="422" t="n">
-        <v>1.90669</v>
+        <v>1</v>
       </c>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
@@ -5446,11 +5446,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n"/>
-      <c r="E9" s="339" t="n"/>
-      <c r="F9" s="339" t="n"/>
-      <c r="G9" s="339" t="n"/>
-      <c r="H9" s="422" t="n"/>
+      <c r="D9" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E9" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G9" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H9" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5505,11 +5515,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n"/>
-      <c r="E10" s="339" t="n"/>
-      <c r="F10" s="339" t="n"/>
-      <c r="G10" s="339" t="n"/>
-      <c r="H10" s="422" t="n"/>
+      <c r="D10" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E10" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G10" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H10" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5564,11 +5584,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n"/>
-      <c r="E11" s="339" t="n"/>
-      <c r="F11" s="339" t="n"/>
-      <c r="G11" s="339" t="n"/>
-      <c r="H11" s="422" t="n"/>
+      <c r="D11" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E11" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G11" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H11" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5623,11 +5653,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n"/>
-      <c r="E12" s="339" t="n"/>
-      <c r="F12" s="339" t="n"/>
-      <c r="G12" s="339" t="n"/>
-      <c r="H12" s="422" t="n"/>
+      <c r="D12" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E12" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G12" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H12" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5682,11 +5722,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n"/>
-      <c r="E13" s="343" t="n"/>
-      <c r="F13" s="343" t="n"/>
-      <c r="G13" s="343" t="n"/>
-      <c r="H13" s="424" t="n"/>
+      <c r="D13" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E13" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="343" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G13" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H13" s="424" t="n">
+        <v>1</v>
+      </c>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5741,11 +5791,21 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n"/>
-      <c r="E14" s="344" t="n"/>
-      <c r="F14" s="344" t="n"/>
-      <c r="G14" s="344" t="n"/>
-      <c r="H14" s="426" t="n"/>
+      <c r="D14" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E14" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G14" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H14" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5800,11 +5860,21 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n"/>
-      <c r="E15" s="344" t="n"/>
-      <c r="F15" s="344" t="n"/>
-      <c r="G15" s="344" t="n"/>
-      <c r="H15" s="426" t="n"/>
+      <c r="D15" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E15" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G15" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H15" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5859,11 +5929,21 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n"/>
-      <c r="E16" s="344" t="n"/>
-      <c r="F16" s="344" t="n"/>
-      <c r="G16" s="344" t="n"/>
-      <c r="H16" s="426" t="n"/>
+      <c r="D16" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E16" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G16" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H16" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5918,11 +5998,21 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n"/>
-      <c r="E17" s="344" t="n"/>
-      <c r="F17" s="344" t="n"/>
-      <c r="G17" s="344" t="n"/>
-      <c r="H17" s="426" t="n"/>
+      <c r="D17" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E17" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G17" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H17" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -5977,11 +6067,21 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n"/>
-      <c r="E18" s="344" t="n"/>
-      <c r="F18" s="344" t="n"/>
-      <c r="G18" s="344" t="n"/>
-      <c r="H18" s="426" t="n"/>
+      <c r="D18" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E18" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G18" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H18" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6036,11 +6136,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n"/>
-      <c r="E19" s="343" t="n"/>
-      <c r="F19" s="343" t="n"/>
-      <c r="G19" s="343" t="n"/>
-      <c r="H19" s="424" t="n"/>
+      <c r="D19" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E19" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G19" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H19" s="424" t="n">
+        <v>1</v>
+      </c>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6566,21 +6676,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E29" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="419" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G29" s="419" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H29" s="420" t="n">
-        <v>1</v>
-      </c>
+      <c r="D29" s="418" t="n"/>
+      <c r="E29" s="419" t="n"/>
+      <c r="F29" s="419" t="n"/>
+      <c r="G29" s="419" t="n"/>
+      <c r="H29" s="420" t="n"/>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
         <v/>
@@ -6635,21 +6735,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E30" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G30" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H30" s="422" t="n">
-        <v>1</v>
-      </c>
+      <c r="D30" s="421" t="n"/>
+      <c r="E30" s="339" t="n"/>
+      <c r="F30" s="339" t="n"/>
+      <c r="G30" s="339" t="n"/>
+      <c r="H30" s="422" t="n"/>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
         <v/>
@@ -6704,21 +6794,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E31" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G31" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H31" s="422" t="n">
-        <v>1</v>
-      </c>
+      <c r="D31" s="421" t="n"/>
+      <c r="E31" s="339" t="n"/>
+      <c r="F31" s="339" t="n"/>
+      <c r="G31" s="339" t="n"/>
+      <c r="H31" s="422" t="n"/>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
         <v/>
@@ -6773,21 +6853,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E32" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G32" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H32" s="422" t="n">
-        <v>1</v>
-      </c>
+      <c r="D32" s="421" t="n"/>
+      <c r="E32" s="339" t="n"/>
+      <c r="F32" s="339" t="n"/>
+      <c r="G32" s="339" t="n"/>
+      <c r="H32" s="422" t="n"/>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
         <v/>
@@ -6842,21 +6912,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E33" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G33" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H33" s="422" t="n">
-        <v>1</v>
-      </c>
+      <c r="D33" s="421" t="n"/>
+      <c r="E33" s="339" t="n"/>
+      <c r="F33" s="339" t="n"/>
+      <c r="G33" s="339" t="n"/>
+      <c r="H33" s="422" t="n"/>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
         <v/>
@@ -6911,21 +6971,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E34" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G34" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H34" s="422" t="n">
-        <v>1</v>
-      </c>
+      <c r="D34" s="421" t="n"/>
+      <c r="E34" s="339" t="n"/>
+      <c r="F34" s="339" t="n"/>
+      <c r="G34" s="339" t="n"/>
+      <c r="H34" s="422" t="n"/>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
         <v/>
@@ -6980,21 +7030,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E35" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="343" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G35" s="343" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H35" s="424" t="n">
-        <v>1</v>
-      </c>
+      <c r="D35" s="423" t="n"/>
+      <c r="E35" s="343" t="n"/>
+      <c r="F35" s="343" t="n"/>
+      <c r="G35" s="343" t="n"/>
+      <c r="H35" s="424" t="n"/>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
         <v/>
@@ -7049,21 +7089,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E36" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G36" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H36" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D36" s="425" t="n"/>
+      <c r="E36" s="344" t="n"/>
+      <c r="F36" s="344" t="n"/>
+      <c r="G36" s="344" t="n"/>
+      <c r="H36" s="426" t="n"/>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
         <v/>
@@ -7118,21 +7148,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E37" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G37" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H37" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D37" s="425" t="n"/>
+      <c r="E37" s="344" t="n"/>
+      <c r="F37" s="344" t="n"/>
+      <c r="G37" s="344" t="n"/>
+      <c r="H37" s="426" t="n"/>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
         <v/>

</xml_diff>

<commit_message>
merge con QT develop
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -5315,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G7" s="419" t="n">
         <v>-1.3734</v>
@@ -5453,7 +5453,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G9" s="339" t="n">
         <v>-1.3734</v>
@@ -5657,7 +5657,7 @@
         <v>837</v>
       </c>
       <c r="E12" s="339" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F12" s="339" t="n">
         <v>-156.5579745837849</v>
@@ -5726,10 +5726,10 @@
         <v>837</v>
       </c>
       <c r="E13" s="343" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F13" s="343" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G13" s="343" t="n">
         <v>-1.3734</v>
@@ -5795,10 +5795,10 @@
         <v>837</v>
       </c>
       <c r="E14" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F14" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G14" s="344" t="n">
         <v>-1.3734</v>
@@ -5864,10 +5864,10 @@
         <v>837</v>
       </c>
       <c r="E15" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F15" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G15" s="344" t="n">
         <v>-1.3734</v>
@@ -5929,21 +5929,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E16" s="344" t="n">
-        <v>800</v>
-      </c>
-      <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G16" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H16" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D16" s="425" t="n"/>
+      <c r="E16" s="344" t="n"/>
+      <c r="F16" s="344" t="n"/>
+      <c r="G16" s="344" t="n"/>
+      <c r="H16" s="426" t="n"/>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5998,21 +5988,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E17" s="344" t="n">
-        <v>800</v>
-      </c>
-      <c r="F17" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G17" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H17" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D17" s="425" t="n"/>
+      <c r="E17" s="344" t="n"/>
+      <c r="F17" s="344" t="n"/>
+      <c r="G17" s="344" t="n"/>
+      <c r="H17" s="426" t="n"/>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -6067,21 +6047,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E18" s="344" t="n">
-        <v>800</v>
-      </c>
-      <c r="F18" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G18" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H18" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D18" s="425" t="n"/>
+      <c r="E18" s="344" t="n"/>
+      <c r="F18" s="344" t="n"/>
+      <c r="G18" s="344" t="n"/>
+      <c r="H18" s="426" t="n"/>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6136,21 +6106,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E19" s="343" t="n">
-        <v>800</v>
-      </c>
-      <c r="F19" s="343" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G19" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H19" s="424" t="n">
-        <v>1</v>
-      </c>
+      <c r="D19" s="423" t="n"/>
+      <c r="E19" s="343" t="n"/>
+      <c r="F19" s="343" t="n"/>
+      <c r="G19" s="343" t="n"/>
+      <c r="H19" s="424" t="n"/>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6683,7 +6643,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G29" s="419" t="n">
         <v>-1.3734</v>
@@ -6890,7 +6850,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G32" s="339" t="n">
         <v>-1.3734</v>
@@ -6959,7 +6919,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G33" s="339" t="n">
         <v>-1.3734</v>
@@ -7297,21 +7257,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D38" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E38" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G38" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H38" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D38" s="425" t="n"/>
+      <c r="E38" s="344" t="n"/>
+      <c r="F38" s="344" t="n"/>
+      <c r="G38" s="344" t="n"/>
+      <c r="H38" s="426" t="n"/>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7366,21 +7316,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D39" s="425" t="n"/>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7435,21 +7375,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E40" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G40" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H40" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D40" s="425" t="n"/>
+      <c r="E40" s="344" t="n"/>
+      <c r="F40" s="344" t="n"/>
+      <c r="G40" s="344" t="n"/>
+      <c r="H40" s="426" t="n"/>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7504,21 +7434,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E41" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G41" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H41" s="424" t="n">
-        <v>1</v>
-      </c>
+      <c r="D41" s="423" t="n"/>
+      <c r="E41" s="343" t="n"/>
+      <c r="F41" s="343" t="n"/>
+      <c r="G41" s="343" t="n"/>
+      <c r="H41" s="424" t="n"/>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>

</xml_diff>

<commit_message>
prova per grafico di riassunto
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -5315,10 +5315,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H7" s="420" t="n">
         <v>1</v>
@@ -5384,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G8" s="339" t="n">
         <v>-1.3734</v>
@@ -5522,10 +5522,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G10" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H10" s="422" t="n">
         <v>1</v>
@@ -5594,7 +5594,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G11" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H11" s="422" t="n">
         <v>1</v>
@@ -5657,13 +5657,13 @@
         <v>837</v>
       </c>
       <c r="E12" s="339" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F12" s="339" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G12" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H12" s="422" t="n">
         <v>1</v>
@@ -5726,7 +5726,7 @@
         <v>837</v>
       </c>
       <c r="E13" s="343" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F13" s="343" t="n">
         <v>-157.0411782090434</v>
@@ -5795,13 +5795,13 @@
         <v>837</v>
       </c>
       <c r="E14" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F14" s="344" t="n">
         <v>-157.0411782090434</v>
       </c>
       <c r="G14" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H14" s="426" t="n">
         <v>1</v>
@@ -5864,13 +5864,13 @@
         <v>837</v>
       </c>
       <c r="E15" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F15" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G15" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H15" s="426" t="n">
         <v>1</v>
@@ -5933,13 +5933,13 @@
         <v>837</v>
       </c>
       <c r="E16" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G16" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H16" s="426" t="n">
         <v>1</v>
@@ -6002,13 +6002,13 @@
         <v>837</v>
       </c>
       <c r="E17" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F17" s="344" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G17" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H17" s="426" t="n">
         <v>1</v>
@@ -6071,13 +6071,13 @@
         <v>837</v>
       </c>
       <c r="E18" s="344" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F18" s="344" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G18" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H18" s="426" t="n">
         <v>1</v>
@@ -6140,13 +6140,13 @@
         <v>837</v>
       </c>
       <c r="E19" s="343" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="F19" s="343" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G19" s="343" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H19" s="424" t="n">
         <v>1</v>
@@ -6205,11 +6205,21 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D20" s="425" t="n"/>
-      <c r="E20" s="344" t="n"/>
-      <c r="F20" s="344" t="n"/>
-      <c r="G20" s="344" t="n"/>
-      <c r="H20" s="426" t="n"/>
+      <c r="D20" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E20" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G20" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H20" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I20" s="365">
         <f>(H20-$E$5)+$H$2</f>
         <v/>
@@ -6264,11 +6274,21 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D21" s="425" t="n"/>
-      <c r="E21" s="344" t="n"/>
-      <c r="F21" s="344" t="n"/>
-      <c r="G21" s="344" t="n"/>
-      <c r="H21" s="426" t="n"/>
+      <c r="D21" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E21" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G21" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H21" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I21" s="365">
         <f>(H21-$E$5)+$H$2</f>
         <v/>
@@ -6323,11 +6343,21 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D22" s="425" t="n"/>
-      <c r="E22" s="344" t="n"/>
-      <c r="F22" s="344" t="n"/>
-      <c r="G22" s="344" t="n"/>
-      <c r="H22" s="426" t="n"/>
+      <c r="D22" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E22" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G22" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H22" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I22" s="365">
         <f>(H22-$E$5)+$H$2</f>
         <v/>
@@ -6382,11 +6412,21 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D23" s="425" t="n"/>
-      <c r="E23" s="344" t="n"/>
-      <c r="F23" s="344" t="n"/>
-      <c r="G23" s="344" t="n"/>
-      <c r="H23" s="426" t="n"/>
+      <c r="D23" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E23" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G23" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H23" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I23" s="365">
         <f>(H23-$E$5)+$H$2</f>
         <v/>
@@ -6441,11 +6481,21 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D24" s="427" t="n"/>
-      <c r="E24" s="348" t="n"/>
-      <c r="F24" s="348" t="n"/>
-      <c r="G24" s="348" t="n"/>
-      <c r="H24" s="428" t="n"/>
+      <c r="D24" s="427" t="n">
+        <v>837</v>
+      </c>
+      <c r="E24" s="348" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="348" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G24" s="348" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H24" s="428" t="n">
+        <v>1</v>
+      </c>
       <c r="I24" s="366">
         <f>(H24-$E$5)+$H$2</f>
         <v/>
@@ -6500,11 +6550,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D25" s="429" t="n"/>
-      <c r="E25" s="430" t="n"/>
-      <c r="F25" s="430" t="n"/>
-      <c r="G25" s="430" t="n"/>
-      <c r="H25" s="431" t="n"/>
+      <c r="D25" s="429" t="n">
+        <v>837</v>
+      </c>
+      <c r="E25" s="430" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="430" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G25" s="430" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H25" s="431" t="n">
+        <v>1</v>
+      </c>
       <c r="I25" s="366">
         <f>(H25-$E$5)+$H$2</f>
         <v/>
@@ -6683,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G29" s="419" t="n">
         <v>-1.3734</v>
@@ -6755,7 +6815,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G30" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H30" s="422" t="n">
         <v>1</v>
@@ -6824,7 +6884,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G31" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H31" s="422" t="n">
         <v>1</v>
@@ -6890,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G32" s="339" t="n">
         <v>-1.3734</v>
@@ -6962,7 +7022,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G33" s="339" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H33" s="422" t="n">
         <v>1</v>
@@ -7100,7 +7160,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G35" s="343" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H35" s="424" t="n">
         <v>1</v>
@@ -7169,7 +7229,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G36" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H36" s="426" t="n">
         <v>1</v>
@@ -7235,10 +7295,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G37" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H37" s="426" t="n">
         <v>1</v>
@@ -7307,7 +7367,7 @@
         <v>-157.0411782090434</v>
       </c>
       <c r="G38" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H38" s="426" t="n">
         <v>1</v>
@@ -7376,7 +7436,7 @@
         <v>-156.5579745837849</v>
       </c>
       <c r="G39" s="344" t="n">
-        <v>-1.3734</v>
+        <v>-1.1772</v>
       </c>
       <c r="H39" s="426" t="n">
         <v>1</v>
@@ -7442,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G40" s="344" t="n">
         <v>-1.3734</v>
@@ -7573,11 +7633,21 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D42" s="425" t="n"/>
-      <c r="E42" s="344" t="n"/>
-      <c r="F42" s="344" t="n"/>
-      <c r="G42" s="344" t="n"/>
-      <c r="H42" s="426" t="n"/>
+      <c r="D42" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E42" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G42" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H42" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I42" s="365">
         <f>(H42-$E$27)+$H$2</f>
         <v/>
@@ -7632,11 +7702,21 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D43" s="425" t="n"/>
-      <c r="E43" s="344" t="n"/>
-      <c r="F43" s="344" t="n"/>
-      <c r="G43" s="344" t="n"/>
-      <c r="H43" s="426" t="n"/>
+      <c r="D43" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E43" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G43" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H43" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I43" s="365">
         <f>(H43-$E$27)+$H$2</f>
         <v/>
@@ -7691,11 +7771,21 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D44" s="425" t="n"/>
-      <c r="E44" s="344" t="n"/>
-      <c r="F44" s="344" t="n"/>
-      <c r="G44" s="344" t="n"/>
-      <c r="H44" s="426" t="n"/>
+      <c r="D44" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E44" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G44" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H44" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I44" s="365">
         <f>(H44-$E$27)+$H$2</f>
         <v/>
@@ -7750,11 +7840,21 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D45" s="425" t="n"/>
-      <c r="E45" s="344" t="n"/>
-      <c r="F45" s="344" t="n"/>
-      <c r="G45" s="344" t="n"/>
-      <c r="H45" s="426" t="n"/>
+      <c r="D45" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E45" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G45" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H45" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I45" s="365">
         <f>(H45-$E$27)+$H$2</f>
         <v/>
@@ -7809,11 +7909,21 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D46" s="425" t="n"/>
-      <c r="E46" s="344" t="n"/>
-      <c r="F46" s="344" t="n"/>
-      <c r="G46" s="344" t="n"/>
-      <c r="H46" s="426" t="n"/>
+      <c r="D46" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E46" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G46" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H46" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I46" s="366">
         <f>(H46-$E$27)+$H$2</f>
         <v/>
@@ -7868,11 +7978,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D47" s="429" t="n"/>
-      <c r="E47" s="430" t="n"/>
-      <c r="F47" s="430" t="n"/>
-      <c r="G47" s="430" t="n"/>
-      <c r="H47" s="431" t="n"/>
+      <c r="D47" s="429" t="n">
+        <v>837</v>
+      </c>
+      <c r="E47" s="430" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="430" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G47" s="430" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H47" s="431" t="n">
+        <v>1</v>
+      </c>
       <c r="I47" s="366">
         <f>(H47-$E$27)+$H$2</f>
         <v/>
@@ -8859,11 +8979,11 @@
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="B50:H51"/>
     <mergeCell ref="B60:B61"/>
-    <mergeCell ref="G60:H60"/>
     <mergeCell ref="A74:A85"/>
     <mergeCell ref="C74:D74"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="E60:F60"/>
     <mergeCell ref="A60:A71"/>
-    <mergeCell ref="E60:F60"/>
     <mergeCell ref="E74:F74"/>
     <mergeCell ref="G74:H74"/>
     <mergeCell ref="K50:Q51"/>
@@ -9131,7 +9251,7 @@
         <v/>
       </c>
       <c r="B13" s="6" t="n">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="E13" s="9" t="inlineStr">
         <is>
@@ -9236,7 +9356,7 @@
         <v/>
       </c>
       <c r="B20" s="6" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
@@ -10209,8 +10329,10 @@
           <t>Data:</t>
         </is>
       </c>
-      <c r="B63" s="526" t="n">
-        <v>45476</v>
+      <c r="B63" s="526" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C63" s="52" t="n"/>
     </row>
@@ -10222,7 +10344,7 @@
       </c>
       <c r="B64" s="54" t="inlineStr">
         <is>
-          <t>E-ELE 2411</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C64" s="52" t="n"/>
@@ -10235,7 +10357,7 @@
       </c>
       <c r="B65" s="54" t="inlineStr">
         <is>
-          <t>Dallara</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C65" s="52" t="inlineStr">
@@ -10252,7 +10374,7 @@
       </c>
       <c r="B66" s="54" t="inlineStr">
         <is>
-          <t>E03F008A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C66" s="52" t="inlineStr">
@@ -10269,7 +10391,7 @@
       </c>
       <c r="B67" s="54" t="inlineStr">
         <is>
-          <t>Clutch-Shaft Hewland Toyota Yaris</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -10289,7 +10411,11 @@
           <t>Progetto UUT:</t>
         </is>
       </c>
-      <c r="B68" s="54" t="n"/>
+      <c r="B68" s="54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C68" s="52" t="inlineStr">
         <is>
           <t>M189 PVP #30</t>
@@ -25619,8 +25745,8 @@
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F16:M16"/>
+    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G70:H70"/>
-    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G97:H97"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>

</xml_diff>

<commit_message>
grafico di aggiornamento concluso
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -5312,16 +5312,16 @@
         <v>837</v>
       </c>
       <c r="E7" s="419" t="n">
-        <v>989</v>
+        <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-0.3</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-2.4</v>
+        <v>-1.1772</v>
       </c>
       <c r="H7" s="420" t="n">
-        <v>2.42215</v>
+        <v>1</v>
       </c>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
@@ -5381,16 +5381,16 @@
         <v>837</v>
       </c>
       <c r="E8" s="339" t="n">
-        <v>883</v>
+        <v>0</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>257</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G8" s="339" t="n">
-        <v>-253.9</v>
+        <v>-1.1772</v>
       </c>
       <c r="H8" s="422" t="n">
-        <v>1.90669</v>
+        <v>1</v>
       </c>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
@@ -5446,11 +5446,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n"/>
-      <c r="E9" s="339" t="n"/>
-      <c r="F9" s="339" t="n"/>
-      <c r="G9" s="339" t="n"/>
-      <c r="H9" s="422" t="n"/>
+      <c r="D9" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E9" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G9" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H9" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5505,11 +5515,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n"/>
-      <c r="E10" s="339" t="n"/>
-      <c r="F10" s="339" t="n"/>
-      <c r="G10" s="339" t="n"/>
-      <c r="H10" s="422" t="n"/>
+      <c r="D10" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E10" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G10" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H10" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5564,11 +5584,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n"/>
-      <c r="E11" s="339" t="n"/>
-      <c r="F11" s="339" t="n"/>
-      <c r="G11" s="339" t="n"/>
-      <c r="H11" s="422" t="n"/>
+      <c r="D11" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E11" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="339" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G11" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H11" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5623,11 +5653,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n"/>
-      <c r="E12" s="339" t="n"/>
-      <c r="F12" s="339" t="n"/>
-      <c r="G12" s="339" t="n"/>
-      <c r="H12" s="422" t="n"/>
+      <c r="D12" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E12" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G12" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H12" s="422" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5682,11 +5722,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n"/>
-      <c r="E13" s="343" t="n"/>
-      <c r="F13" s="343" t="n"/>
-      <c r="G13" s="343" t="n"/>
-      <c r="H13" s="424" t="n"/>
+      <c r="D13" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E13" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="343" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G13" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H13" s="424" t="n">
+        <v>1</v>
+      </c>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5741,11 +5791,21 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n"/>
-      <c r="E14" s="344" t="n"/>
-      <c r="F14" s="344" t="n"/>
-      <c r="G14" s="344" t="n"/>
-      <c r="H14" s="426" t="n"/>
+      <c r="D14" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E14" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G14" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H14" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5800,11 +5860,21 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n"/>
-      <c r="E15" s="344" t="n"/>
-      <c r="F15" s="344" t="n"/>
-      <c r="G15" s="344" t="n"/>
-      <c r="H15" s="426" t="n"/>
+      <c r="D15" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E15" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G15" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H15" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5859,11 +5929,21 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n"/>
-      <c r="E16" s="344" t="n"/>
-      <c r="F16" s="344" t="n"/>
-      <c r="G16" s="344" t="n"/>
-      <c r="H16" s="426" t="n"/>
+      <c r="D16" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E16" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G16" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H16" s="426" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -6573,7 +6653,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G29" s="419" t="n">
         <v>-1.1772</v>
@@ -6642,7 +6722,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G30" s="339" t="n">
         <v>-1.1772</v>
@@ -6711,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G31" s="339" t="n">
         <v>-1.1772</v>
@@ -6780,7 +6860,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G32" s="339" t="n">
         <v>-1.1772</v>
@@ -6849,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G33" s="339" t="n">
         <v>-1.1772</v>
@@ -6918,7 +6998,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G34" s="339" t="n">
         <v>-1.1772</v>
@@ -7125,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G37" s="344" t="n">
         <v>-1.1772</v>
@@ -7256,21 +7336,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>1</v>
-      </c>
+      <c r="D39" s="425" t="n"/>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -25495,9 +25565,9 @@
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F16:M16"/>
-    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G70:H70"/>
     <mergeCell ref="G97:H97"/>
+    <mergeCell ref="L102:L103"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I91:J91"/>

</xml_diff>

<commit_message>
small change in read me
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Test.xlsx
@@ -5321,7 +5321,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H7" s="420" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
@@ -5384,13 +5384,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G8" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H8" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
@@ -5453,13 +5453,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G9" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H9" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
@@ -5528,7 +5528,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H10" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
@@ -5591,13 +5591,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G11" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H11" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
@@ -5660,13 +5660,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="339" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G12" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H12" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
@@ -5729,13 +5729,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="343" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G13" s="343" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H13" s="424" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
@@ -5798,13 +5798,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G14" s="344" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H14" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
@@ -5867,13 +5867,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G15" s="344" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H15" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
@@ -5936,13 +5936,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G16" s="344" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H16" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
@@ -5998,11 +5998,21 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n"/>
-      <c r="E17" s="344" t="n"/>
-      <c r="F17" s="344" t="n"/>
-      <c r="G17" s="344" t="n"/>
-      <c r="H17" s="426" t="n"/>
+      <c r="D17" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E17" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G17" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H17" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -6057,11 +6067,21 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n"/>
-      <c r="E18" s="344" t="n"/>
-      <c r="F18" s="344" t="n"/>
-      <c r="G18" s="344" t="n"/>
-      <c r="H18" s="426" t="n"/>
+      <c r="D18" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E18" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G18" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H18" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6116,11 +6136,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n"/>
-      <c r="E19" s="343" t="n"/>
-      <c r="F19" s="343" t="n"/>
-      <c r="G19" s="343" t="n"/>
-      <c r="H19" s="424" t="n"/>
+      <c r="D19" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E19" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G19" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H19" s="424" t="n">
+        <v>500</v>
+      </c>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6175,11 +6205,21 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D20" s="425" t="n"/>
-      <c r="E20" s="344" t="n"/>
-      <c r="F20" s="344" t="n"/>
-      <c r="G20" s="344" t="n"/>
-      <c r="H20" s="426" t="n"/>
+      <c r="D20" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E20" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G20" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H20" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I20" s="365">
         <f>(H20-$E$5)+$H$2</f>
         <v/>
@@ -6234,11 +6274,21 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D21" s="425" t="n"/>
-      <c r="E21" s="344" t="n"/>
-      <c r="F21" s="344" t="n"/>
-      <c r="G21" s="344" t="n"/>
-      <c r="H21" s="426" t="n"/>
+      <c r="D21" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E21" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G21" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H21" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I21" s="365">
         <f>(H21-$E$5)+$H$2</f>
         <v/>
@@ -6659,7 +6709,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H29" s="420" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
@@ -6722,13 +6772,13 @@
         <v>0</v>
       </c>
       <c r="F30" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G30" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H30" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
@@ -6797,7 +6847,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H31" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
@@ -6866,7 +6916,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H32" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
@@ -6935,7 +6985,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H33" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
@@ -6998,13 +7048,13 @@
         <v>0</v>
       </c>
       <c r="F34" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G34" s="339" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H34" s="422" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
@@ -7067,13 +7117,13 @@
         <v>0</v>
       </c>
       <c r="F35" s="343" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G35" s="343" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H35" s="424" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
@@ -7142,7 +7192,7 @@
         <v>-1.1772</v>
       </c>
       <c r="H36" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
@@ -7205,13 +7255,13 @@
         <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G37" s="344" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H37" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
@@ -7274,13 +7324,13 @@
         <v>0</v>
       </c>
       <c r="F38" s="344" t="n">
-        <v>-157.0411782090434</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G38" s="344" t="n">
         <v>-1.1772</v>
       </c>
       <c r="H38" s="426" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
@@ -7336,11 +7386,21 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n"/>
-      <c r="E39" s="344" t="n"/>
-      <c r="F39" s="344" t="n"/>
-      <c r="G39" s="344" t="n"/>
-      <c r="H39" s="426" t="n"/>
+      <c r="D39" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E39" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G39" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H39" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7395,11 +7455,21 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n"/>
-      <c r="E40" s="344" t="n"/>
-      <c r="F40" s="344" t="n"/>
-      <c r="G40" s="344" t="n"/>
-      <c r="H40" s="426" t="n"/>
+      <c r="D40" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E40" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G40" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H40" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7454,11 +7524,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n"/>
-      <c r="E41" s="343" t="n"/>
-      <c r="F41" s="343" t="n"/>
-      <c r="G41" s="343" t="n"/>
-      <c r="H41" s="424" t="n"/>
+      <c r="D41" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E41" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G41" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H41" s="424" t="n">
+        <v>500</v>
+      </c>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -7513,11 +7593,21 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D42" s="425" t="n"/>
-      <c r="E42" s="344" t="n"/>
-      <c r="F42" s="344" t="n"/>
-      <c r="G42" s="344" t="n"/>
-      <c r="H42" s="426" t="n"/>
+      <c r="D42" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E42" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G42" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H42" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I42" s="365">
         <f>(H42-$E$27)+$H$2</f>
         <v/>
@@ -7572,11 +7662,21 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D43" s="425" t="n"/>
-      <c r="E43" s="344" t="n"/>
-      <c r="F43" s="344" t="n"/>
-      <c r="G43" s="344" t="n"/>
-      <c r="H43" s="426" t="n"/>
+      <c r="D43" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E43" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G43" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H43" s="426" t="n">
+        <v>500</v>
+      </c>
       <c r="I43" s="365">
         <f>(H43-$E$27)+$H$2</f>
         <v/>
@@ -9071,7 +9171,7 @@
         <v/>
       </c>
       <c r="B13" s="6" t="n">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E13" s="9" t="inlineStr">
         <is>
@@ -10175,11 +10275,7 @@
           <t>Cliente:</t>
         </is>
       </c>
-      <c r="B65" s="54" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="B65" s="54" t="inlineStr"/>
       <c r="C65" s="52" t="inlineStr">
         <is>
           <t>Maserati</t>
@@ -25565,9 +25661,9 @@
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F16:M16"/>
+    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G70:H70"/>
     <mergeCell ref="G97:H97"/>
-    <mergeCell ref="L102:L103"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I91:J91"/>

</xml_diff>